<commit_message>
Update the old ATACseq
</commit_message>
<xml_diff>
--- a/atacseq/v2.0.0/atacseq-v2.0.0.xlsx
+++ b/atacseq/v2.0.0/atacseq-v2.0.0.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="378">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -479,12 +479,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000202</t>
   </si>
   <si>
-    <t>RNAseq (Visium)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000188</t>
-  </si>
-  <si>
     <t>Cell DIVE</t>
   </si>
   <si>
@@ -497,6 +491,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000160</t>
   </si>
   <si>
+    <t>GeoMx (NGS)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -509,12 +509,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
-    <t>GeoMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000216</t>
-  </si>
-  <si>
     <t>RNAseq (bulk)</t>
   </si>
   <si>
@@ -533,12 +527,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>RNAseq (GeoMx)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000214</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -575,6 +563,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
   </si>
   <si>
+    <t>GeoMx (nCounter)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
+  </si>
+  <si>
     <t>PhenoCycler</t>
   </si>
   <si>
@@ -1196,6 +1190,12 @@
     <t>http://purl.obolibrary.org/obo/UO_0010050</t>
   </si>
   <si>
+    <t>nM</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000065</t>
+  </si>
+  <si>
     <t>library_layout</t>
   </si>
   <si>
@@ -1508,7 +1508,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-07T20:05:53-08:00</t>
+    <t>2023-11-22T10:19:45-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1698,82 +1698,82 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K1" t="s" s="1">
+        <v>216</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>217</v>
+      </c>
+      <c r="M1" t="s" s="1">
         <v>218</v>
       </c>
-      <c r="L1" t="s" s="1">
+      <c r="N1" t="s" s="1">
         <v>219</v>
       </c>
-      <c r="M1" t="s" s="1">
+      <c r="O1" t="s" s="1">
         <v>220</v>
       </c>
-      <c r="N1" t="s" s="1">
-        <v>221</v>
-      </c>
-      <c r="O1" t="s" s="1">
-        <v>222</v>
-      </c>
       <c r="P1" t="s" s="1">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="R1" t="s" s="1">
+        <v>239</v>
+      </c>
+      <c r="S1" t="s" s="1">
+        <v>240</v>
+      </c>
+      <c r="T1" t="s" s="1">
         <v>241</v>
       </c>
-      <c r="S1" t="s" s="1">
-        <v>242</v>
-      </c>
-      <c r="T1" t="s" s="1">
-        <v>243</v>
-      </c>
       <c r="U1" t="s" s="1">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="V1" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="W1" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="X1" t="s" s="1">
         <v>258</v>
       </c>
-      <c r="W1" t="s" s="1">
+      <c r="Y1" t="s" s="1">
         <v>259</v>
       </c>
-      <c r="X1" t="s" s="1">
+      <c r="Z1" t="s" s="1">
         <v>260</v>
       </c>
-      <c r="Y1" t="s" s="1">
-        <v>261</v>
-      </c>
-      <c r="Z1" t="s" s="1">
-        <v>262</v>
-      </c>
       <c r="AA1" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="AB1" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="AC1" t="s" s="1">
         <v>265</v>
       </c>
-      <c r="AB1" t="s" s="1">
+      <c r="AD1" t="s" s="1">
         <v>266</v>
-      </c>
-      <c r="AC1" t="s" s="1">
-        <v>267</v>
-      </c>
-      <c r="AD1" t="s" s="1">
-        <v>268</v>
       </c>
       <c r="AE1" t="s" s="1">
         <v>271</v>
@@ -1835,7 +1835,7 @@
   </sheetData>
   <dataValidations count="36">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$35</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$11</formula1>
@@ -1873,7 +1873,7 @@
       <formula1>'barcode_size'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_offset'!$A$1:$A$2</formula1>
+      <formula1>'umi_offset'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'umi_read'!$A$1:$A$3</formula1>
@@ -1911,7 +1911,7 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AD2:AD1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_concentration_unit'!$A$1:$A$1</formula1>
+      <formula1>'library_concentration_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AE2:AE1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'library_layout'!$A$1:$A$2</formula1>
@@ -1968,26 +1968,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2005,32 +2005,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2040,7 +2040,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2048,12 +2048,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2071,26 +2076,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2108,27 +2113,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2146,42 +2151,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2199,10 +2204,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2220,10 +2225,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2233,7 +2238,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2241,9 +2246,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>269</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -2283,7 +2296,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2559,14 +2572,6 @@
       </c>
       <c r="B34" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2661,10 +2666,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -2698,12 +2703,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2846,10 +2851,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2912,18 +2917,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4">
@@ -2944,10 +2949,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7">
@@ -2973,18 +2978,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -3005,18 +3010,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7">
@@ -3174,90 +3179,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3275,12 +3280,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3298,114 +3303,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3423,306 +3428,306 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3740,42 +3745,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3793,26 +3798,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3830,32 +3835,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>